<commit_message>
Updated Practicum Paper Trial and Excel Files
</commit_message>
<xml_diff>
--- a/Excel Output/AllAsia.xlsx
+++ b/Excel Output/AllAsia.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26722" uniqueCount="1058">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26722" uniqueCount="1059">
   <si>
     <t>Time</t>
   </si>
@@ -3234,6 +3234,9 @@
   </si>
   <si>
     <t>1985-89</t>
+  </si>
+  <si>
+    <t>1980-84</t>
   </si>
 </sst>
 </file>
@@ -7733,7 +7736,7 @@
         <v>661</v>
       </c>
       <c r="K10" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="L10" t="s">
         <v>672</v>
@@ -7940,10 +7943,10 @@
         <v>1051</v>
       </c>
       <c r="CB10" t="s">
-        <v>1050</v>
+        <v>1051</v>
       </c>
       <c r="CC10" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="CD10" t="s">
         <v>1051</v>
@@ -85767,7 +85770,7 @@
         <v>1051</v>
       </c>
       <c r="FG168" t="s">
-        <v>964</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="169">

</xml_diff>